<commit_message>
Compiled all data and regressions into one unified model
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1760,67 +1760,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.71197795776191597</c:v>
+                  <c:v>0.73224494636710946</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76881140561455497</c:v>
+                  <c:v>0.80133999060750472</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82020980068514371</c:v>
+                  <c:v>0.864851191658492</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.86297960819861808</c:v>
+                  <c:v>0.91889795794664175</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.89235411398931619</c:v>
+                  <c:v>0.95694431549519887</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.90300000000000002</c:v>
+                  <c:v>0.97069496317210635</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.89235411398931619</c:v>
+                  <c:v>0.95592039089463432</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.86297960819861808</c:v>
+                  <c:v>0.91713413531726418</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.82020980068514371</c:v>
+                  <c:v>0.86263892023268907</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.76881140561455497</c:v>
+                  <c:v>0.79886567271366205</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.71197795776191597</c:v>
+                  <c:v>0.72961307228564687</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.65165496154625013</c:v>
+                  <c:v>0.65699289127139959</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.5890149637162746</c:v>
+                  <c:v>0.58220119539941184</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.52478054117183881</c:v>
+                  <c:v>0.5059447263683341</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.45941177544773693</c:v>
+                  <c:v>0.42866062697939855</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.39321175931071217</c:v>
+                  <c:v>0.35063102349393183</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.3263866660925544</c:v>
+                  <c:v>0.27204497853226861</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.25908086647983886</c:v>
+                  <c:v>0.19303341166414456</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.19139809861573198</c:v>
+                  <c:v>0.11368959777842447</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12341462891251487</c:v>
+                  <c:v>3.408165787335582E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.5187675060959895E-2</c:v>
+                  <c:v>-4.5739568782209972E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8339,67 +8339,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>0.72189752875566504</c:v>
+                  <c:v>0.68546895273516073</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.77453505248499444</c:v>
+                  <c:v>0.75403360694673549</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.82150842871606322</c:v>
+                  <c:v>0.81735427248960968</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.85991128768001679</c:v>
+                  <c:v>0.87162116796561739</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.88576612086364759</c:v>
+                  <c:v>0.91017963724211881</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.89499999999999991</c:v>
+                  <c:v>0.924224841961927</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.88576612086364759</c:v>
+                  <c:v>0.90913649172572497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.85991128768001679</c:v>
+                  <c:v>0.86984218494912913</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.82150842871606322</c:v>
+                  <c:v>0.81514191461878016</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.77453505248499444</c:v>
+                  <c:v>0.75157346456781693</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.72189752875566504</c:v>
+                  <c:v>0.68286196051215287</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.66549304613581128</c:v>
+                  <c:v>0.61102682242418116</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.60652410903450604</c:v>
+                  <c:v>0.53719304096181131</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.54575883477335918</c:v>
+                  <c:v>0.46201811679758253</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.48369904516568807</c:v>
+                  <c:v>0.38590570997273166</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.42068159064465527</c:v>
+                  <c:v>0.30911497109292407</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.35693883014052141</c:v>
+                  <c:v>0.23181890410459449</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.29263520672354892</c:v>
+                  <c:v>0.15413696757324513</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.22788985732517208</c:v>
+                  <c:v>7.6154085728904253E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.16279093897826113</c:v>
+                  <c:v>-2.0678244257792411E-3</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9.7404934434990542E-2</c:v>
+                  <c:v>-8.048261604547724E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8408,6 +8408,362 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-DD53-4425-8D8D-3B98BDD41E19}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$19:$H$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.1875</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.391111111151986</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.116944444365799</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.117499999993015</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.82361111114733</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$19:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.74283431301116942</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.81945131549835204</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78519902954101561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69956825504302977</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.37777678499221801</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15333401987552642</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A8BB-462D-9BDB-C26AF2F73B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$26:$H$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.990833333460614</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43.387777777912561</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>69.113333333458286</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>94.115833333460614</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.95861111109843</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$26:$E$31</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.82395820150375365</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.9690798355102539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88525180349349974</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.74734119901657103</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.40481810102462767</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1614464057445526</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A8BB-462D-9BDB-C26AF2F73B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$33:$H$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.993333333346527</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.58416666672565</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.263888889050577</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.34805555571802</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>111.92972222232493</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$33:$E$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.66351316699981688</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87713943252563475</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90057520399093627</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.59771267900466918</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21372625062465667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6457296440601345E-2</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-A8BB-462D-9BDB-C26AF2F73B9A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$40:$H$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.991388888796791</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>41.585833333258051</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>67.262500000011642</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90.348888888896909</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>112.0191666665487</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$40:$E$45</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.6806393099784851</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78429762849807738</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.78880451450347899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56346039304733275</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.21733176538944243</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1253913475036621</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A8BB-462D-9BDB-C26AF2F73B9A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -8421,414 +8777,7 @@
         </c:dLbls>
         <c:axId val="456542520"/>
         <c:axId val="456544816"/>
-        <c:extLst>
-          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="3"/>
-                <c:order val="3"/>
-                <c:spPr>
-                  <a:ln w="25400" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent4"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent4"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$19:$H$24</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>18.1875</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>43.391111111151986</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>69.116944444365799</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>94.117499999993015</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>112.82361111114733</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst>
-                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$19:$E$24</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0.74283431301116942</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.81945131549835204</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.78519902954101561</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.69956825504302977</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.37777678499221801</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.15333401987552642</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst>
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000000-A8BB-462D-9BDB-C26AF2F73B9A}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="4"/>
-                <c:order val="4"/>
-                <c:spPr>
-                  <a:ln w="25400" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent5"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$26:$H$31</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>17.990833333460614</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>43.387777777912561</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>69.113333333458286</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>94.115833333460614</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>112.95861111109843</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$26:$E$31</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0.82395820150375365</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.9690798355102539</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.88525180349349974</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.74734119901657103</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.40481810102462767</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.1614464057445526</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-A8BB-462D-9BDB-C26AF2F73B9A}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="5"/>
-                <c:order val="5"/>
-                <c:spPr>
-                  <a:ln w="25400" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent6"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent6"/>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$33:$H$38</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>20.993333333346527</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>41.58416666672565</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>67.263888889050577</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>90.34805555571802</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>111.92972222232493</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$33:$E$38</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0.66351316699981688</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.87713943252563475</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.90057520399093627</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.59771267900466918</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.21372625062465667</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>9.6457296440601345E-2</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-A8BB-462D-9BDB-C26AF2F73B9A}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-            <c15:filteredScatterSeries>
-              <c15:ser>
-                <c:idx val="6"/>
-                <c:order val="6"/>
-                <c:spPr>
-                  <a:ln w="25400" cap="rnd">
-                    <a:noFill/>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="circle"/>
-                  <c:size val="5"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent1">
-                        <a:lumMod val="60000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent1">
-                          <a:lumMod val="60000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c:marker>
-                <c:xVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$H$40:$H$45</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>20.991388888796791</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>41.585833333258051</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>67.262500000011642</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>90.348888888896909</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>112.0191666665487</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:xVal>
-                <c:yVal>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>Sheet1!$E$40:$E$45</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>0.00</c:formatCode>
-                      <c:ptCount val="6"/>
-                      <c:pt idx="0">
-                        <c:v>0.6806393099784851</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0.78429762849807738</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0.78880451450347899</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0.56346039304733275</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0.21733176538944243</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0.1253913475036621</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:yVal>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-A8BB-462D-9BDB-C26AF2F73B9A}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredScatterSeries>
-          </c:ext>
-        </c:extLst>
+        <c:extLst/>
       </c:scatterChart>
       <c:valAx>
         <c:axId val="456542520"/>
@@ -10896,67 +10845,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2.0128923567376709</c:v>
+                  <c:v>2.0350163019622984</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2380903352722386</c:v>
+                  <c:v>2.2576864155513561</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4583256202126251</c:v>
+                  <c:v>2.475511422972978</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6724569264291973</c:v>
+                  <c:v>2.6873916050579427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8790135901708278</c:v>
+                  <c:v>2.8919140090058861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0760944918407032</c:v>
+                  <c:v>3.0872574176207066</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2612462008493903</c:v>
+                  <c:v>3.2710777114246063</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.431332976398878</c:v>
+                  <c:v>3.440384684492892</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5824360684830543</c:v>
+                  <c:v>3.5914433924127862</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.7098627502068604</c:v>
+                  <c:v>3.7197715939620295</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.8083962818073513</c:v>
+                  <c:v>3.8203519750603321</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8729239833912823</c:v>
+                  <c:v>3.8881898479465642</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8994429776952622</c:v>
+                  <c:v>3.9192362442055906</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8861305194304672</c:v>
+                  <c:v>3.9114200629864793</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8339154951268708</c:v>
+                  <c:v>3.8652767189011992</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7461805630556881</c:v>
+                  <c:v>3.7837790412611172</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.6277933756099721</c:v>
+                  <c:v>3.6714817292894395</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4840268438749247</c:v>
+                  <c:v>3.5334809550512043</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3197924773771881</c:v>
+                  <c:v>3.3746251318715244</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1392767991603678</c:v>
+                  <c:v>3.1991078818296601</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.9458686203169457</c:v>
+                  <c:v>3.0103584003922133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11216,7 +11165,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'D401'!$I$3:$I$23</c15:sqref>
@@ -11294,7 +11243,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'D401'!$L$3:$L$23</c15:sqref>
@@ -11305,73 +11254,73 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="21"/>
                       <c:pt idx="0">
-                        <c:v>1.7632296951433557</c:v>
+                        <c:v>1.7854331654394877</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2.004340921604256</c:v>
+                        <c:v>2.023837899500653</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>2.2401387738207292</c:v>
+                        <c:v>2.2570551558678993</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2.4694013196105318</c:v>
+                        <c:v>2.4839075055102073</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>2.6905539731667516</c:v>
+                        <c:v>2.7028821516216546</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>2.9015612753763924</c:v>
+                        <c:v>2.9120291836628076</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.0997964279781893</c:v>
+                        <c:v>3.1088388387754895</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>3.281902108164044</c:v>
+                        <c:v>3.2901096130094185</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.4436826538489056</c:v>
+                        <c:v>3.4518426381954059</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>3.5801137342440321</c:v>
+                        <c:v>3.5892389428443399</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>3.6856099771779869</c:v>
+                        <c:v>3.6969266725581038</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>3.7546974235700348</c:v>
+                        <c:v>3.769558198109686</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>3.7830903393623974</c:v>
+                        <c:v>3.8027984373334847</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>3.7688371779427374</c:v>
+                        <c:v>3.7944299384142495</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>3.7129324640929489</c:v>
+                        <c:v>3.7450259501644103</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>3.6189978861149341</c:v>
+                        <c:v>3.6577693720308768</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>3.4922450611204972</c:v>
+                        <c:v>3.5375367536301869</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>3.3383195018582219</c:v>
+                        <c:v>3.3897843797161058</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>3.1624797816663288</c:v>
+                        <c:v>3.2197032688351337</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>2.9692082574124035</c:v>
+                        <c:v>3.031783378532289</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>2.7621332049986957</c:v>
+                        <c:v>2.8296962227798845</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-DE1E-42B8-8024-6229A4067695}"/>
                   </c:ext>
@@ -11415,7 +11364,7 @@
                 </c:marker>
                 <c:xVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'D401'!$I$3:$I$23</c15:sqref>
@@ -11493,7 +11442,7 @@
                 </c:xVal>
                 <c:yVal>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'D401'!$M$3:$M$23</c15:sqref>
@@ -11504,73 +11453,73 @@
                       <c:formatCode>General</c:formatCode>
                       <c:ptCount val="21"/>
                       <c:pt idx="0">
-                        <c:v>2.2625550183319856</c:v>
+                        <c:v>2.2845994384851096</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>2.4718397489402206</c:v>
+                        <c:v>2.4915349316020592</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>2.676512466604521</c:v>
+                        <c:v>2.6939676900780567</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>2.8755125332478628</c:v>
+                        <c:v>2.8908757046056781</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>3.067473207174904</c:v>
+                        <c:v>3.0809458663901177</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>3.2506277083050139</c:v>
+                        <c:v>3.2624856515786052</c:v>
                       </c:pt>
                       <c:pt idx="6">
-                        <c:v>3.4226959737205913</c:v>
+                        <c:v>3.4333165840737236</c:v>
                       </c:pt>
                       <c:pt idx="7">
-                        <c:v>3.5807638446337124</c:v>
+                        <c:v>3.5906597559763647</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>3.7211894831172039</c:v>
+                        <c:v>3.7310441466301665</c:v>
                       </c:pt>
                       <c:pt idx="9">
-                        <c:v>3.8396117661696887</c:v>
+                        <c:v>3.8503042450797187</c:v>
                       </c:pt>
                       <c:pt idx="10">
-                        <c:v>3.9311825864367163</c:v>
+                        <c:v>3.9437772775625604</c:v>
                       </c:pt>
                       <c:pt idx="11">
-                        <c:v>3.9911505432125294</c:v>
+                        <c:v>4.0068214977834424</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>4.015795616028127</c:v>
+                        <c:v>4.0356740510776961</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>4.0034238609181969</c:v>
+                        <c:v>4.0284101875587091</c:v>
                       </c:pt>
                       <c:pt idx="14">
-                        <c:v>3.9548985261607927</c:v>
+                        <c:v>3.985527487637988</c:v>
                       </c:pt>
                       <c:pt idx="15">
-                        <c:v>3.8733632399964417</c:v>
+                        <c:v>3.9097887104913571</c:v>
                       </c:pt>
                       <c:pt idx="16">
-                        <c:v>3.7633416900994474</c:v>
+                        <c:v>3.8054267049486925</c:v>
                       </c:pt>
                       <c:pt idx="17">
-                        <c:v>3.6297341858916279</c:v>
+                        <c:v>3.6771775303863032</c:v>
                       </c:pt>
                       <c:pt idx="18">
-                        <c:v>3.4771051730880473</c:v>
+                        <c:v>3.529546994907915</c:v>
                       </c:pt>
                       <c:pt idx="19">
-                        <c:v>3.3093453409083327</c:v>
+                        <c:v>3.3664323851270317</c:v>
                       </c:pt>
                       <c:pt idx="20">
-                        <c:v>3.1296040356351962</c:v>
+                        <c:v>3.1910205780045415</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:yVal>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-DE1E-42B8-8024-6229A4067695}"/>
                   </c:ext>
@@ -12645,67 +12594,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.5452026497595297</c:v>
+                  <c:v>1.5310308253843257</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6376943283880874</c:v>
+                  <c:v>1.6041735873137231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.7297581355862586</c:v>
+                  <c:v>1.6768845057213064</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.8211653704042383</c:v>
+                  <c:v>1.7489560660003618</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.9114936813323122</c:v>
+                  <c:v>1.820027135979615</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.9998772675969128</c:v>
+                  <c:v>1.8894167175335406</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.0842756194959033</c:v>
+                  <c:v>1.9557052863459128</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.1589612412162196</c:v>
+                  <c:v>2.015573172538109</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.2062296322321391</c:v>
+                  <c:v>2.0606732779975716</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.1955158981264606</c:v>
+                  <c:v>2.0743962837557239</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.1358373290096999</c:v>
+                  <c:v>2.0481617755201427</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.0568105468063442</c:v>
+                  <c:v>1.9966876746758306</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.9707194418119127</c:v>
+                  <c:v>1.9340973869713949</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1.8815438191362173</c:v>
+                  <c:v>1.8665384198769313</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1.7907896031097921</c:v>
+                  <c:v>1.796480487065421</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.6991291768511267</c:v>
+                  <c:v>1.7250211575952579</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.6069033062123106</c:v>
+                  <c:v>1.6527061030059103</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.5143019002972915</c:v>
+                  <c:v>1.5798331585813787</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.4214387745324335</c:v>
+                  <c:v>1.5065774333705615</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.328386144410868</c:v>
+                  <c:v>1.433048176656381</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1.2351919788309982</c:v>
+                  <c:v>1.3593169024319933</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13147,67 +13096,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>2.0128923567376709</c:v>
+                  <c:v>2.0350163019622984</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2380903352722386</c:v>
+                  <c:v>2.2576864155513561</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4583256202126251</c:v>
+                  <c:v>2.475511422972978</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6724569264291973</c:v>
+                  <c:v>2.6873916050579427</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.8790135901708278</c:v>
+                  <c:v>2.8919140090058861</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.0760944918407032</c:v>
+                  <c:v>3.0872574176207066</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.2612462008493903</c:v>
+                  <c:v>3.2710777114246063</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.431332976398878</c:v>
+                  <c:v>3.440384684492892</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.5824360684830543</c:v>
+                  <c:v>3.5914433924127862</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.7098627502068604</c:v>
+                  <c:v>3.7197715939620295</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.8083962818073513</c:v>
+                  <c:v>3.8203519750603321</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.8729239833912823</c:v>
+                  <c:v>3.8881898479465642</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.8994429776952622</c:v>
+                  <c:v>3.9192362442055906</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.8861305194304672</c:v>
+                  <c:v>3.9114200629864793</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.8339154951268708</c:v>
+                  <c:v>3.8652767189011992</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7461805630556881</c:v>
+                  <c:v>3.7837790412611172</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.6277933756099721</c:v>
+                  <c:v>3.6714817292894395</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3.4840268438749247</c:v>
+                  <c:v>3.5334809550512043</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.3197924773771881</c:v>
+                  <c:v>3.3746251318715244</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3.1392767991603678</c:v>
+                  <c:v>3.1991078818296601</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.9458686203169457</c:v>
+                  <c:v>3.0103584003922133</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15363,67 +15312,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.4391275155102359</c:v>
+                  <c:v>1.3988835148375665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6689641421115926</c:v>
+                  <c:v>1.6300846113976495</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.893426774844198</c:v>
+                  <c:v>1.8560544685585634</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1113095900063295</c:v>
+                  <c:v>2.0756245356561784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3210716903285906</c:v>
+                  <c:v>2.2873014797471156</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5207409738164319</c:v>
+                  <c:v>2.48917281578969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7078025372322232</c:v>
+                  <c:v>2.678795740218769</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8790869277056084</c:v>
+                  <c:v>2.853082227896742</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0306971407069945</c:v>
+                  <c:v>3.008215394599465</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1580504905085829</c:v>
+                  <c:v>3.1396682535181455</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.256149231873902</c:v>
+                  <c:v>3.2424363967172853</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3201846807021438</c:v>
+                  <c:v>3.3115983352273637</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.3464486798520374</c:v>
+                  <c:v>3.3432053032922178</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3332682314705986</c:v>
+                  <c:v>3.3352508186464638</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.28149472490579</c:v>
+                  <c:v>3.2882527472808203</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.1942496824568636</c:v>
+                  <c:v>3.2050972568462859</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0760859632682824</c:v>
+                  <c:v>3.0902431338049703</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.932023244372751</c:v>
+                  <c:v>2.9487357504144338</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.766827536661709</c:v>
+                  <c:v>2.7854354696879993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5846377533161493</c:v>
+                  <c:v>2.604598314095945</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3888614431761361</c:v>
+                  <c:v>2.4097440394497833</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15772,67 +15721,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.4391275155102359</c:v>
+                  <c:v>1.3988835148375665</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.6689641421115926</c:v>
+                  <c:v>1.6300846113976495</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.893426774844198</c:v>
+                  <c:v>1.8560544685585634</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1113095900063295</c:v>
+                  <c:v>2.0756245356561784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3210716903285906</c:v>
+                  <c:v>2.2873014797471156</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5207409738164319</c:v>
+                  <c:v>2.48917281578969</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.7078025372322232</c:v>
+                  <c:v>2.678795740218769</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8790869277056084</c:v>
+                  <c:v>2.853082227896742</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.0306971407069945</c:v>
+                  <c:v>3.008215394599465</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1580504905085829</c:v>
+                  <c:v>3.1396682535181455</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.256149231873902</c:v>
+                  <c:v>3.2424363967172853</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3.3201846807021438</c:v>
+                  <c:v>3.3115983352273637</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.3464486798520374</c:v>
+                  <c:v>3.3432053032922178</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.3332682314705986</c:v>
+                  <c:v>3.3352508186464638</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.28149472490579</c:v>
+                  <c:v>3.2882527472808203</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.1942496824568636</c:v>
+                  <c:v>3.2050972568462859</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0760859632682824</c:v>
+                  <c:v>3.0902431338049703</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.932023244372751</c:v>
+                  <c:v>2.9487357504144338</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.766827536661709</c:v>
+                  <c:v>2.7854354696879993</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.5846377533161493</c:v>
+                  <c:v>2.604598314095945</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.3888614431761361</c:v>
+                  <c:v>2.4097440394497833</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -16124,67 +16073,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>1.8914191718519637</c:v>
+                  <c:v>1.8458732337909605</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1562066371791992</c:v>
+                  <c:v>2.1113306944583621</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4209941025064357</c:v>
+                  <c:v>2.3767881551257637</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6857815678336712</c:v>
+                  <c:v>2.6422456157931653</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.9505690331609076</c:v>
+                  <c:v>2.9077030764605669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.2153564984881431</c:v>
+                  <c:v>3.1731605371279685</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.4801439638153795</c:v>
+                  <c:v>3.4386179977953701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.744931429142615</c:v>
+                  <c:v>3.7040754584627718</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.0097188944698505</c:v>
+                  <c:v>3.9695329191301725</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.2745063597970869</c:v>
+                  <c:v>4.2349903797975745</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.5392938251243233</c:v>
+                  <c:v>4.5004478404649753</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.804081290451558</c:v>
+                  <c:v>4.7659053011323778</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0688687557787944</c:v>
+                  <c:v>5.0313627617997785</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.3336562211060308</c:v>
+                  <c:v>5.296820222467181</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.5984436864332654</c:v>
+                  <c:v>5.5622776831345817</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.8632311517605018</c:v>
+                  <c:v>5.8277351438019842</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6.1280186170877382</c:v>
+                  <c:v>6.0931926044693849</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6.3928060824149728</c:v>
+                  <c:v>6.3586500651367857</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>6.657593547742211</c:v>
+                  <c:v>6.6241075258041882</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.9223810130694456</c:v>
+                  <c:v>6.8895649864715907</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.187168478396682</c:v>
+                  <c:v>7.1550224471389914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -25646,16 +25595,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -26462,8 +26411,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE72"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2:AE2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26575,19 +26524,19 @@
       </c>
       <c r="Z2">
         <f>$AE$2+$AB$2*SQRT(1+(Y2-$AD$2)^2/($AC$2)^2)</f>
-        <v>0.71197795776191597</v>
+        <v>0.73224494636710946</v>
       </c>
       <c r="AB2">
-        <v>-0.224</v>
+        <v>-0.2243</v>
       </c>
       <c r="AC2">
-        <v>19.234000000000002</v>
+        <v>16.563099999999999</v>
       </c>
       <c r="AD2">
-        <v>30</v>
+        <v>29.888999999999999</v>
       </c>
       <c r="AE2">
-        <v>1.127</v>
+        <v>1.1950000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.25">
@@ -26616,7 +26565,7 @@
       </c>
       <c r="Z3">
         <f t="shared" ref="Z3:Z22" si="0">$AE$2+$AB$2*SQRT(1+(Y3-$AD$2)^2/($AC$2)^2)</f>
-        <v>0.76881140561455497</v>
+        <v>0.80133999060750472</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
@@ -26645,7 +26594,7 @@
       </c>
       <c r="Z4">
         <f t="shared" si="0"/>
-        <v>0.82020980068514371</v>
+        <v>0.864851191658492</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.25">
@@ -26674,7 +26623,7 @@
       </c>
       <c r="Z5">
         <f t="shared" si="0"/>
-        <v>0.86297960819861808</v>
+        <v>0.91889795794664175</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.25">
@@ -26703,7 +26652,7 @@
       </c>
       <c r="Z6">
         <f t="shared" si="0"/>
-        <v>0.89235411398931619</v>
+        <v>0.95694431549519887</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.25">
@@ -26731,7 +26680,7 @@
       </c>
       <c r="Z7">
         <f t="shared" si="0"/>
-        <v>0.90300000000000002</v>
+        <v>0.97069496317210635</v>
       </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.25">
@@ -26744,7 +26693,7 @@
       </c>
       <c r="Z8">
         <f t="shared" si="0"/>
-        <v>0.89235411398931619</v>
+        <v>0.95592039089463432</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.25">
@@ -26772,7 +26721,7 @@
       </c>
       <c r="Z9">
         <f t="shared" si="0"/>
-        <v>0.86297960819861808</v>
+        <v>0.91713413531726418</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.25">
@@ -26800,7 +26749,7 @@
       </c>
       <c r="Z10">
         <f t="shared" si="0"/>
-        <v>0.82020980068514371</v>
+        <v>0.86263892023268907</v>
       </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.25">
@@ -26828,7 +26777,7 @@
       </c>
       <c r="Z11">
         <f t="shared" si="0"/>
-        <v>0.76881140561455497</v>
+        <v>0.79886567271366205</v>
       </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.25">
@@ -26856,7 +26805,7 @@
       </c>
       <c r="Z12">
         <f t="shared" si="0"/>
-        <v>0.71197795776191597</v>
+        <v>0.72961307228564687</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.25">
@@ -26884,7 +26833,7 @@
       </c>
       <c r="Z13">
         <f t="shared" si="0"/>
-        <v>0.65165496154625013</v>
+        <v>0.65699289127139959</v>
       </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.25">
@@ -26912,7 +26861,7 @@
       </c>
       <c r="Z14">
         <f t="shared" si="0"/>
-        <v>0.5890149637162746</v>
+        <v>0.58220119539941184</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.25">
@@ -26924,7 +26873,7 @@
       </c>
       <c r="Z15">
         <f t="shared" si="0"/>
-        <v>0.52478054117183881</v>
+        <v>0.5059447263683341</v>
       </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.25">
@@ -26992,7 +26941,7 @@
       </c>
       <c r="Z16">
         <f t="shared" si="0"/>
-        <v>0.45941177544773693</v>
+        <v>0.42866062697939855</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
@@ -27060,7 +27009,7 @@
       </c>
       <c r="Z17">
         <f t="shared" si="0"/>
-        <v>0.39321175931071217</v>
+        <v>0.35063102349393183</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -27128,7 +27077,7 @@
       </c>
       <c r="Z18">
         <f t="shared" si="0"/>
-        <v>0.3263866660925544</v>
+        <v>0.27204497853226861</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -27199,7 +27148,7 @@
       </c>
       <c r="Z19">
         <f t="shared" si="0"/>
-        <v>0.25908086647983886</v>
+        <v>0.19303341166414456</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -27270,7 +27219,7 @@
       </c>
       <c r="Z20">
         <f t="shared" si="0"/>
-        <v>0.19139809861573198</v>
+        <v>0.11368959777842447</v>
       </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
@@ -27341,7 +27290,7 @@
       </c>
       <c r="Z21">
         <f t="shared" si="0"/>
-        <v>0.12341462891251487</v>
+        <v>3.408165787335582E-2</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -27412,7 +27361,7 @@
       </c>
       <c r="Z22">
         <f t="shared" si="0"/>
-        <v>5.5187675060959895E-2</v>
+        <v>-4.5739568782209972E-2</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -29098,7 +29047,7 @@
   <dimension ref="B1:AO50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W3" sqref="T3:W3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29237,11 +29186,11 @@
       </c>
       <c r="K3">
         <f>$W$3+$T$3*SQRT(1+(H3-$V$3)^2/($U$3)^2)</f>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="L3">
         <f>(E3-K3)^2</f>
-        <v>1.5567299062843893E-3</v>
+        <v>9.1617644464039637E-6</v>
       </c>
       <c r="M3" s="4">
         <f>AVERAGE(E3:E45)</f>
@@ -29252,22 +29201,22 @@
       </c>
       <c r="P3">
         <f>$W$3+$T$3*SQRT(1+(O3-$V$3)^2/($U$3)^2)</f>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="S3" t="s">
         <v>184</v>
       </c>
       <c r="T3">
-        <v>-0.24099999999999999</v>
+        <v>-0.21077000000000001</v>
       </c>
       <c r="U3">
-        <v>-21.47</v>
+        <v>15.866</v>
       </c>
       <c r="V3">
-        <v>30</v>
+        <v>29.888999999999999</v>
       </c>
       <c r="W3">
-        <v>1.1359999999999999</v>
+        <v>1.135</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" ref="AA3:AA18" si="0">24*(AC3-$AC$2)</f>
@@ -29336,18 +29285,18 @@
       </c>
       <c r="K4">
         <f t="shared" ref="K4:K45" si="3">$W$3+$T$3*SQRT(1+(H4-$V$3)^2/($U$3)^2)</f>
-        <v>0.84088633843450022</v>
+        <v>0.84437228398465347</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L45" si="4">(E4-K4)^2</f>
-        <v>4.2162962805331104E-4</v>
+        <v>5.7693962016627332E-4</v>
       </c>
       <c r="O4">
         <v>6</v>
       </c>
       <c r="P4">
         <f t="shared" ref="P4:P23" si="5">$W$3+$T$3*SQRT(1+(O4-$V$3)^2/($U$3)^2)</f>
-        <v>0.77453505248499444</v>
+        <v>0.75403360694673549</v>
       </c>
       <c r="S4" t="s">
         <v>185</v>
@@ -29431,18 +29380,18 @@
       </c>
       <c r="K5">
         <f t="shared" si="3"/>
-        <v>0.87294880807012754</v>
+        <v>0.89081620946539009</v>
       </c>
       <c r="L5">
         <f t="shared" si="4"/>
-        <v>1.1949844767596739E-3</v>
+        <v>2.7495287373048953E-3</v>
       </c>
       <c r="O5">
         <v>12</v>
       </c>
       <c r="P5">
         <f t="shared" si="5"/>
-        <v>0.82150842871606322</v>
+        <v>0.81735427248960968</v>
       </c>
       <c r="AA5" s="4">
         <f t="shared" si="0"/>
@@ -29514,18 +29463,18 @@
       </c>
       <c r="K6">
         <f t="shared" si="3"/>
-        <v>0.87442110075592283</v>
+        <v>0.89155226189742709</v>
       </c>
       <c r="L6">
         <f t="shared" si="4"/>
-        <v>1.4321412609335428E-3</v>
+        <v>3.0222290111123753E-3</v>
       </c>
       <c r="O6">
         <v>18</v>
       </c>
       <c r="P6">
         <f t="shared" si="5"/>
-        <v>0.85991128768001679</v>
+        <v>0.87162116796561739</v>
       </c>
       <c r="T6" t="s">
         <v>317</v>
@@ -29603,18 +29552,18 @@
       </c>
       <c r="K7">
         <f t="shared" si="3"/>
-        <v>0.6791707458933357</v>
+        <v>0.62831755510205023</v>
       </c>
       <c r="L7">
         <f t="shared" si="4"/>
-        <v>3.3715285014425329E-4</v>
+        <v>1.0556955170724367E-3</v>
       </c>
       <c r="O7">
         <v>24</v>
       </c>
       <c r="P7">
         <f t="shared" si="5"/>
-        <v>0.88576612086364759</v>
+        <v>0.91017963724211881</v>
       </c>
       <c r="AA7" s="4">
         <f t="shared" si="0"/>
@@ -29686,18 +29635,18 @@
       </c>
       <c r="K8">
         <f t="shared" si="3"/>
-        <v>0.45023600176137979</v>
+        <v>0.3450758675629686</v>
       </c>
       <c r="L8">
         <f t="shared" si="4"/>
-        <v>2.3580313437240607E-5</v>
+        <v>1.0060928065668252E-2</v>
       </c>
       <c r="O8">
         <v>30</v>
       </c>
       <c r="P8">
         <f t="shared" si="5"/>
-        <v>0.89499999999999991</v>
+        <v>0.924224841961927</v>
       </c>
       <c r="AA8" s="4">
         <f t="shared" si="0"/>
@@ -29769,18 +29718,18 @@
       </c>
       <c r="K9">
         <f t="shared" si="3"/>
-        <v>0.19129547170064043</v>
+        <v>3.2162306495291393E-2</v>
       </c>
       <c r="L9">
         <f t="shared" si="4"/>
-        <v>2.8870127862352796E-6</v>
+        <v>2.5867024344119787E-2</v>
       </c>
       <c r="O9">
         <v>36</v>
       </c>
       <c r="P9">
         <f t="shared" si="5"/>
-        <v>0.88576612086364759</v>
+        <v>0.90913649172572497</v>
       </c>
       <c r="AA9" s="4">
         <f t="shared" si="0"/>
@@ -29833,7 +29782,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="5"/>
-        <v>0.85991128768001679</v>
+        <v>0.86984218494912913</v>
       </c>
       <c r="AA10" s="4">
         <f t="shared" si="0"/>
@@ -29905,18 +29854,18 @@
       </c>
       <c r="K11">
         <f t="shared" si="3"/>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="L11">
         <f t="shared" si="4"/>
-        <v>7.2017946841198513E-4</v>
+        <v>9.2014450519842966E-5</v>
       </c>
       <c r="O11">
         <v>48</v>
       </c>
       <c r="P11">
         <f t="shared" si="5"/>
-        <v>0.82150842871606322</v>
+        <v>0.81514191461878016</v>
       </c>
       <c r="AA11" s="4">
         <f t="shared" si="0"/>
@@ -29988,18 +29937,18 @@
       </c>
       <c r="K12">
         <f t="shared" si="3"/>
-        <v>0.84144315561504834</v>
+        <v>0.84515871015650201</v>
       </c>
       <c r="L12">
         <f t="shared" si="4"/>
-        <v>2.5118416258070077E-3</v>
+        <v>2.1532125926412835E-3</v>
       </c>
       <c r="O12">
         <v>54</v>
       </c>
       <c r="P12">
         <f t="shared" si="5"/>
-        <v>0.77453505248499444</v>
+        <v>0.75157346456781693</v>
       </c>
       <c r="AA12" s="4">
         <f t="shared" si="0"/>
@@ -30071,18 +30020,18 @@
       </c>
       <c r="K13">
         <f t="shared" si="3"/>
-        <v>0.87252591026948567</v>
+        <v>0.89018594478361879</v>
       </c>
       <c r="L13">
         <f t="shared" si="4"/>
-        <v>6.7552079659603762E-5</v>
+        <v>8.9132996394766038E-5</v>
       </c>
       <c r="O13">
         <v>60</v>
       </c>
       <c r="P13">
         <f t="shared" si="5"/>
-        <v>0.72189752875566504</v>
+        <v>0.68286196051215287</v>
       </c>
       <c r="AA13" s="4">
         <f t="shared" si="0"/>
@@ -30154,18 +30103,18 @@
       </c>
       <c r="K14">
         <f t="shared" si="3"/>
-        <v>0.87469064772902105</v>
+        <v>0.89196302683758544</v>
       </c>
       <c r="L14">
         <f t="shared" si="4"/>
-        <v>1.036469369473118E-3</v>
+        <v>2.2266206237886411E-4</v>
       </c>
       <c r="O14">
         <v>66</v>
       </c>
       <c r="P14">
         <f t="shared" si="5"/>
-        <v>0.66549304613581128</v>
+        <v>0.61102682242418116</v>
       </c>
       <c r="AA14" s="4">
         <f t="shared" si="0"/>
@@ -30237,18 +30186,18 @@
       </c>
       <c r="K15">
         <f t="shared" si="3"/>
-        <v>0.67984601128983102</v>
+        <v>0.62917310327798637</v>
       </c>
       <c r="L15">
         <f t="shared" si="4"/>
-        <v>5.4418292703152765E-4</v>
+        <v>5.4760942360764266E-3</v>
       </c>
       <c r="O15">
         <v>72</v>
       </c>
       <c r="P15">
         <f t="shared" si="5"/>
-        <v>0.60652410903450604</v>
+        <v>0.53719304096181131</v>
       </c>
       <c r="AA15" s="4">
         <f t="shared" si="0"/>
@@ -30320,18 +30269,18 @@
       </c>
       <c r="K16">
         <f t="shared" si="3"/>
-        <v>0.45007836482061536</v>
+        <v>0.34488382432265374</v>
       </c>
       <c r="L16">
         <f t="shared" si="4"/>
-        <v>3.1356536947098515E-5</v>
+        <v>9.9191340882894309E-3</v>
       </c>
       <c r="O16">
         <v>78</v>
       </c>
       <c r="P16">
         <f t="shared" si="5"/>
-        <v>0.54575883477335918</v>
+        <v>0.46201811679758253</v>
       </c>
       <c r="AA16" s="4">
         <f t="shared" si="0"/>
@@ -30403,18 +30352,18 @@
       </c>
       <c r="K17">
         <f t="shared" si="3"/>
-        <v>0.19158791182923596</v>
+        <v>3.2513646903878035E-2</v>
       </c>
       <c r="L17">
         <f t="shared" si="4"/>
-        <v>6.6274599612935561E-4</v>
+        <v>3.4157736920544121E-2</v>
       </c>
       <c r="O17">
         <v>84</v>
       </c>
       <c r="P17">
         <f t="shared" si="5"/>
-        <v>0.48369904516568807</v>
+        <v>0.38590570997273166</v>
       </c>
       <c r="AA17" s="4">
         <f t="shared" si="0"/>
@@ -30466,7 +30415,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="5"/>
-        <v>0.42068159064465527</v>
+        <v>0.30911497109292407</v>
       </c>
       <c r="AA18" s="4">
         <f t="shared" si="0"/>
@@ -30538,18 +30487,18 @@
       </c>
       <c r="K19">
         <f t="shared" si="3"/>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="L19">
         <f t="shared" si="4"/>
-        <v>4.3834893496153617E-4</v>
+        <v>3.2907845595962762E-3</v>
       </c>
       <c r="O19">
         <v>96</v>
       </c>
       <c r="P19">
         <f t="shared" si="5"/>
-        <v>0.35693883014052141</v>
+        <v>0.23181890410459449</v>
       </c>
       <c r="AA19" s="4"/>
     </row>
@@ -30579,18 +30528,18 @@
       </c>
       <c r="K20">
         <f t="shared" si="3"/>
-        <v>0.86093199482863314</v>
+        <v>0.8731072308510216</v>
       </c>
       <c r="L20">
         <f t="shared" si="4"/>
-        <v>1.7206467577016097E-3</v>
+        <v>2.878957252332841E-3</v>
       </c>
       <c r="O20">
         <v>102</v>
       </c>
       <c r="P20">
         <f t="shared" si="5"/>
-        <v>0.29263520672354892</v>
+        <v>0.15413696757324513</v>
       </c>
       <c r="AA20" s="4">
         <f>24*(AC20-$AC$20)</f>
@@ -30659,18 +30608,18 @@
       </c>
       <c r="K21">
         <f t="shared" si="3"/>
-        <v>0.85196562637277673</v>
+        <v>0.85823912033123051</v>
       </c>
       <c r="L21">
         <f t="shared" si="4"/>
-        <v>4.4577784524949338E-3</v>
+        <v>5.3348548626428348E-3</v>
       </c>
       <c r="O21">
         <v>108</v>
       </c>
       <c r="P21">
         <f t="shared" si="5"/>
-        <v>0.22788985732517208</v>
+        <v>7.6154085728904253E-2</v>
       </c>
       <c r="AA21" s="4">
         <f t="shared" ref="AA21:AA36" si="8">24*(AC21-$AC$20)</f>
@@ -30739,18 +30688,18 @@
       </c>
       <c r="K22">
         <f t="shared" si="3"/>
-        <v>0.63512295967154431</v>
+        <v>0.57287101863038592</v>
       </c>
       <c r="L22">
         <f t="shared" si="4"/>
-        <v>4.1531960955180063E-3</v>
+        <v>1.6052189714601369E-2</v>
       </c>
       <c r="O22">
         <v>114</v>
       </c>
       <c r="P22">
         <f t="shared" si="5"/>
-        <v>0.16279093897826113</v>
+        <v>-2.0678244257792411E-3</v>
       </c>
       <c r="AA22" s="4">
         <f t="shared" si="8"/>
@@ -30819,18 +30768,18 @@
       </c>
       <c r="K23">
         <f t="shared" si="3"/>
-        <v>0.37700518778214021</v>
+        <v>0.25611689589328723</v>
       </c>
       <c r="L23">
         <f t="shared" si="4"/>
-        <v>5.9536225459984653E-7</v>
+        <v>1.4801128615564135E-2</v>
       </c>
       <c r="O23">
         <v>120</v>
       </c>
       <c r="P23">
         <f t="shared" si="5"/>
-        <v>9.7404934434990542E-2</v>
+        <v>-8.048261604547724E-2</v>
       </c>
       <c r="AA23" s="4">
         <f t="shared" si="8"/>
@@ -30902,11 +30851,11 @@
       </c>
       <c r="K24">
         <f t="shared" si="3"/>
-        <v>0.17557901004406729</v>
+        <v>1.3285210519292434E-2</v>
       </c>
       <c r="L24">
         <f t="shared" si="4"/>
-        <v>4.9483958759847992E-4</v>
+        <v>1.9613669002098773E-2</v>
       </c>
       <c r="AA24" s="4">
         <f t="shared" si="8"/>
@@ -31051,11 +31000,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="3"/>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="L26">
         <f t="shared" si="4"/>
-        <v>1.0416380921792437E-2</v>
+        <v>1.9179272024489217E-2</v>
       </c>
       <c r="O26">
         <v>0</v>
@@ -31159,11 +31108,11 @@
       </c>
       <c r="K27">
         <f t="shared" si="3"/>
-        <v>0.85986107188124183</v>
+        <v>0.87154812712529817</v>
       </c>
       <c r="L27">
         <f t="shared" si="4"/>
-        <v>1.1928738328650008E-2</v>
+        <v>9.5124341404880432E-3</v>
       </c>
       <c r="O27">
         <v>6</v>
@@ -31242,11 +31191,11 @@
       </c>
       <c r="K28">
         <f t="shared" si="3"/>
-        <v>0.85198542593203763</v>
+        <v>0.85826781672372388</v>
       </c>
       <c r="L28">
         <f t="shared" si="4"/>
-        <v>1.10665187606175E-3</v>
+        <v>7.2813554199143912E-4</v>
       </c>
       <c r="O28">
         <v>12</v>
@@ -31343,11 +31292,11 @@
       </c>
       <c r="K29">
         <f t="shared" si="3"/>
-        <v>0.63515849333467345</v>
+        <v>0.57291548997725072</v>
       </c>
       <c r="L29">
         <f t="shared" si="4"/>
-        <v>1.2584959454111257E-2</v>
+        <v>3.0424327973869628E-2</v>
       </c>
       <c r="O29">
         <v>18</v>
@@ -31447,11 +31396,11 @@
       </c>
       <c r="K30">
         <f t="shared" si="3"/>
-        <v>0.37702292787606217</v>
+        <v>0.25613839041301567</v>
       </c>
       <c r="L30">
         <f t="shared" si="4"/>
-        <v>7.7257165035873659E-4</v>
+        <v>2.2105656347552693E-2</v>
       </c>
       <c r="O30">
         <v>24</v>
@@ -31530,11 +31479,11 @@
       </c>
       <c r="K31">
         <f t="shared" si="3"/>
-        <v>0.174112049153753</v>
+        <v>1.1523711985361063E-2</v>
       </c>
       <c r="L31">
         <f t="shared" si="4"/>
-        <v>1.6041852296902153E-4</v>
+        <v>2.2476814104012331E-2</v>
       </c>
       <c r="O31">
         <v>30</v>
@@ -31671,11 +31620,11 @@
       </c>
       <c r="K33">
         <f t="shared" si="3"/>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="L33">
         <f t="shared" si="4"/>
-        <v>3.408733697637745E-3</v>
+        <v>4.8205652725632835E-4</v>
       </c>
       <c r="O33">
         <v>42</v>
@@ -31754,11 +31703,11 @@
       </c>
       <c r="K34">
         <f t="shared" si="3"/>
-        <v>0.87465327114537095</v>
+        <v>0.89336193842888423</v>
       </c>
       <c r="L34">
         <f t="shared" si="4"/>
-        <v>6.1809984087152388E-6</v>
+        <v>2.6316969778096403E-4</v>
       </c>
       <c r="O34">
         <v>48</v>
@@ -31837,11 +31786,11 @@
       </c>
       <c r="K35">
         <f t="shared" si="3"/>
-        <v>0.86215828254302473</v>
+        <v>0.87315716031669344</v>
       </c>
       <c r="L35">
         <f t="shared" si="4"/>
-        <v>1.4758598535350052E-3</v>
+        <v>7.5174911892268736E-4</v>
       </c>
       <c r="O35">
         <v>54</v>
@@ -31920,11 +31869,11 @@
       </c>
       <c r="K36">
         <f t="shared" si="3"/>
-        <v>0.65325363471372966</v>
+        <v>0.59561283223421491</v>
       </c>
       <c r="L36">
         <f t="shared" si="4"/>
-        <v>3.0847977610758181E-3</v>
+        <v>4.4093564593872374E-6</v>
       </c>
       <c r="O36">
         <v>60</v>
@@ -32003,11 +31952,11 @@
       </c>
       <c r="K37">
         <f t="shared" si="3"/>
-        <v>0.4170018886870317</v>
+        <v>0.30464353465403282</v>
       </c>
       <c r="L37">
         <f t="shared" si="4"/>
-        <v>4.1320985029665691E-2</v>
+        <v>8.2659525352782558E-3</v>
       </c>
       <c r="O37">
         <v>66</v>
@@ -32043,11 +31992,11 @@
       </c>
       <c r="K38">
         <f t="shared" si="3"/>
-        <v>0.18528851197309282</v>
+        <v>2.4946218358497196E-2</v>
       </c>
       <c r="L38">
         <f t="shared" si="4"/>
-        <v>7.8909848529799542E-3</v>
+        <v>5.1138342884647966E-3</v>
       </c>
       <c r="O38">
         <v>72</v>
@@ -32092,11 +32041,11 @@
       </c>
       <c r="K40">
         <f t="shared" si="3"/>
-        <v>0.72189752875566504</v>
+        <v>0.68546895273516073</v>
       </c>
       <c r="L40">
         <f t="shared" si="4"/>
-        <v>1.7022406166656437E-3</v>
+        <v>2.3325449157109415E-5</v>
       </c>
       <c r="O40">
         <v>84</v>
@@ -32132,11 +32081,11 @@
       </c>
       <c r="K41">
         <f t="shared" si="3"/>
-        <v>0.87464482706337776</v>
+        <v>0.89334930481729091</v>
       </c>
       <c r="L41">
         <f t="shared" si="4"/>
-        <v>8.1626162885978151E-3</v>
+        <v>1.1892268108030518E-2</v>
       </c>
       <c r="O41">
         <v>90</v>
@@ -32172,11 +32121,11 @@
       </c>
       <c r="K42">
         <f t="shared" si="3"/>
-        <v>0.86214939855234052</v>
+        <v>0.87314402268240721</v>
       </c>
       <c r="L42">
         <f t="shared" si="4"/>
-        <v>5.3794720161409416E-3</v>
+        <v>7.1131526398634992E-3</v>
       </c>
       <c r="O42">
         <v>96</v>
@@ -32212,11 +32161,11 @@
       </c>
       <c r="K43">
         <f t="shared" si="3"/>
-        <v>0.65326714313802658</v>
+        <v>0.59562981577777607</v>
       </c>
       <c r="L43">
         <f t="shared" si="4"/>
-        <v>8.0652523618523365E-3</v>
+        <v>1.0348717588099634E-3</v>
       </c>
       <c r="O43">
         <v>102</v>
@@ -32252,11 +32201,11 @@
       </c>
       <c r="K44">
         <f t="shared" si="3"/>
-        <v>0.41699307567143851</v>
+        <v>0.30463282690103244</v>
       </c>
       <c r="L44">
         <f t="shared" si="4"/>
-        <v>3.9864638823523514E-2</v>
+        <v>7.6214753410504222E-3</v>
       </c>
       <c r="O44">
         <v>108</v>
@@ -32292,11 +32241,11 @@
       </c>
       <c r="K45">
         <f t="shared" si="3"/>
-        <v>0.1843172613183961</v>
+        <v>2.3779596682911297E-2</v>
       </c>
       <c r="L45">
         <f t="shared" si="4"/>
-        <v>3.4722633189014592E-3</v>
+        <v>1.0324947904858351E-2</v>
       </c>
       <c r="O45">
         <v>114</v>
@@ -32322,13 +32271,13 @@
       </c>
       <c r="L48">
         <f>SUM(L3:L45)</f>
-        <v>0.18261258501531538</v>
+        <v>0.31474093127190689</v>
       </c>
     </row>
     <row r="50" spans="11:11" x14ac:dyDescent="0.25">
       <c r="K50">
         <f>1-L48/J48</f>
-        <v>0.93256293194740247</v>
+        <v>0.88376920681922666</v>
       </c>
     </row>
   </sheetData>
@@ -32359,9 +32308,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AG185"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R160" sqref="R160"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A56" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32490,27 +32439,27 @@
       </c>
       <c r="J3">
         <f>$R$3+$O$3*SQRT(1+(I3-$Q$3)^2/$P$3^2)</f>
-        <v>2.0128923567376709</v>
+        <v>2.0350163019622984</v>
       </c>
       <c r="L3">
         <f>$R$9+$O$9*SQRT(1+(I3-$Q$9)^2/$P$9^2)</f>
-        <v>1.7632296951433557</v>
+        <v>1.7854331654394877</v>
       </c>
       <c r="M3">
         <f>$R$10+$O$10*SQRT(1+(I3-$Q$10)^2/$P$10^2)</f>
-        <v>2.2625550183319856</v>
+        <v>2.2845994384851096</v>
       </c>
       <c r="O3">
         <v>-1.6459999999999999</v>
       </c>
       <c r="P3">
-        <v>38.435000000000002</v>
+        <v>38.872</v>
       </c>
       <c r="Q3">
-        <v>73</v>
+        <v>73.8</v>
       </c>
       <c r="R3">
-        <v>5.5460000000000003</v>
+        <v>5.5670000000000002</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
@@ -32538,15 +32487,15 @@
       </c>
       <c r="J4">
         <f t="shared" ref="J4:J22" si="1">$R$3+$O$3*SQRT(1+(I4-$Q$3)^2/$P$3^2)</f>
-        <v>2.2380903352722386</v>
+        <v>2.2576864155513561</v>
       </c>
       <c r="L4">
         <f t="shared" ref="L4:L23" si="2">$R$9+$O$9*SQRT(1+(I4-$Q$9)^2/$P$9^2)</f>
-        <v>2.004340921604256</v>
+        <v>2.023837899500653</v>
       </c>
       <c r="M4">
         <f t="shared" ref="M4:M23" si="3">$R$10+$O$10*SQRT(1+(I4-$Q$10)^2/$P$10^2)</f>
-        <v>2.4718397489402206</v>
+        <v>2.4915349316020592</v>
       </c>
       <c r="O4">
         <v>1.1259999999999999</v>
@@ -32586,15 +32535,15 @@
       </c>
       <c r="J5">
         <f t="shared" si="1"/>
-        <v>2.4583256202126251</v>
+        <v>2.475511422972978</v>
       </c>
       <c r="L5">
         <f t="shared" si="2"/>
-        <v>2.2401387738207292</v>
+        <v>2.2570551558678993</v>
       </c>
       <c r="M5">
         <f t="shared" si="3"/>
-        <v>2.676512466604521</v>
+        <v>2.6939676900780567</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.25">
@@ -32622,15 +32571,15 @@
       </c>
       <c r="J6">
         <f t="shared" si="1"/>
-        <v>2.6724569264291973</v>
+        <v>2.6873916050579427</v>
       </c>
       <c r="L6">
         <f t="shared" si="2"/>
-        <v>2.4694013196105318</v>
+        <v>2.4839075055102073</v>
       </c>
       <c r="M6">
         <f t="shared" si="3"/>
-        <v>2.8755125332478628</v>
+        <v>2.8908757046056781</v>
       </c>
       <c r="O6">
         <f>O3-_xlfn.T.DIST(O3,60,FALSE)*O4</f>
@@ -32638,15 +32587,15 @@
       </c>
       <c r="P6">
         <f t="shared" ref="P6:R6" si="4">P3-_xlfn.T.DIST(P3,60,FALSE)*P4</f>
-        <v>38.435000000000002</v>
+        <v>38.872</v>
       </c>
       <c r="Q6">
         <f t="shared" si="4"/>
-        <v>73</v>
+        <v>73.8</v>
       </c>
       <c r="R6">
         <f t="shared" si="4"/>
-        <v>5.5459986286335798</v>
+        <v>5.5669987319485852</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
@@ -32674,15 +32623,15 @@
       </c>
       <c r="J7">
         <f t="shared" si="1"/>
-        <v>2.8790135901708278</v>
+        <v>2.8919140090058861</v>
       </c>
       <c r="L7">
         <f t="shared" si="2"/>
-        <v>2.6905539731667516</v>
+        <v>2.7028821516216546</v>
       </c>
       <c r="M7">
         <f t="shared" si="3"/>
-        <v>3.067473207174904</v>
+        <v>3.0809458663901177</v>
       </c>
       <c r="O7">
         <f>O3+_xlfn.T.DIST(O3,60,FALSE)*O4</f>
@@ -32690,15 +32639,15 @@
       </c>
       <c r="P7">
         <f t="shared" ref="P7:R7" si="5">P3+_xlfn.T.DIST(P3,60,FALSE)*P4</f>
-        <v>38.435000000000002</v>
+        <v>38.872</v>
       </c>
       <c r="Q7">
         <f t="shared" si="5"/>
-        <v>73</v>
+        <v>73.8</v>
       </c>
       <c r="R7">
         <f t="shared" si="5"/>
-        <v>5.5460013713664207</v>
+        <v>5.5670012680514152</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.25">
@@ -32726,15 +32675,15 @@
       </c>
       <c r="J8">
         <f t="shared" si="1"/>
-        <v>3.0760944918407032</v>
+        <v>3.0872574176207066</v>
       </c>
       <c r="L8">
         <f t="shared" si="2"/>
-        <v>2.9015612753763924</v>
+        <v>2.9120291836628076</v>
       </c>
       <c r="M8">
         <f t="shared" si="3"/>
-        <v>3.2506277083050139</v>
+        <v>3.2624856515786052</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
@@ -32762,15 +32711,15 @@
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>3.2612462008493903</v>
+        <v>3.2710777114246063</v>
       </c>
       <c r="L9">
         <f t="shared" si="2"/>
-        <v>3.0997964279781893</v>
+        <v>3.1088388387754895</v>
       </c>
       <c r="M9">
         <f t="shared" si="3"/>
-        <v>3.4226959737205913</v>
+        <v>3.4333165840737236</v>
       </c>
       <c r="O9">
         <f>O6</f>
@@ -32778,15 +32727,15 @@
       </c>
       <c r="P9">
         <f t="shared" ref="P9:R10" si="6">P6</f>
-        <v>38.435000000000002</v>
+        <v>38.872</v>
       </c>
       <c r="Q9">
         <f t="shared" si="6"/>
-        <v>73</v>
+        <v>73.8</v>
       </c>
       <c r="R9">
         <f t="shared" si="6"/>
-        <v>5.5459986286335798</v>
+        <v>5.5669987319485852</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
@@ -32798,15 +32747,15 @@
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>3.431332976398878</v>
+        <v>3.440384684492892</v>
       </c>
       <c r="L10">
         <f t="shared" si="2"/>
-        <v>3.281902108164044</v>
+        <v>3.2901096130094185</v>
       </c>
       <c r="M10">
         <f t="shared" si="3"/>
-        <v>3.5807638446337124</v>
+        <v>3.5906597559763647</v>
       </c>
       <c r="O10">
         <f>O7</f>
@@ -32814,15 +32763,15 @@
       </c>
       <c r="P10">
         <f t="shared" si="6"/>
-        <v>38.435000000000002</v>
+        <v>38.872</v>
       </c>
       <c r="Q10">
         <f t="shared" si="6"/>
-        <v>73</v>
+        <v>73.8</v>
       </c>
       <c r="R10">
         <f t="shared" si="6"/>
-        <v>5.5460013713664207</v>
+        <v>5.5670012680514152</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
@@ -32850,15 +32799,15 @@
       </c>
       <c r="J11">
         <f t="shared" si="1"/>
-        <v>3.5824360684830543</v>
+        <v>3.5914433924127862</v>
       </c>
       <c r="L11">
         <f t="shared" si="2"/>
-        <v>3.4436826538489056</v>
+        <v>3.4518426381954059</v>
       </c>
       <c r="M11">
         <f t="shared" si="3"/>
-        <v>3.7211894831172039</v>
+        <v>3.7310441466301665</v>
       </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
@@ -32886,15 +32835,15 @@
       </c>
       <c r="J12">
         <f t="shared" si="1"/>
-        <v>3.7098627502068604</v>
+        <v>3.7197715939620295</v>
       </c>
       <c r="L12">
         <f t="shared" si="2"/>
-        <v>3.5801137342440321</v>
+        <v>3.5892389428443399</v>
       </c>
       <c r="M12">
         <f t="shared" si="3"/>
-        <v>3.8396117661696887</v>
+        <v>3.8503042450797187</v>
       </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
@@ -32922,15 +32871,15 @@
       </c>
       <c r="J13">
         <f t="shared" si="1"/>
-        <v>3.8083962818073513</v>
+        <v>3.8203519750603321</v>
       </c>
       <c r="L13">
         <f t="shared" si="2"/>
-        <v>3.6856099771779869</v>
+        <v>3.6969266725581038</v>
       </c>
       <c r="M13">
         <f t="shared" si="3"/>
-        <v>3.9311825864367163</v>
+        <v>3.9437772775625604</v>
       </c>
       <c r="O13">
         <v>-0.38500000000000001</v>
@@ -32970,15 +32919,15 @@
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>3.8729239833912823</v>
+        <v>3.8881898479465642</v>
       </c>
       <c r="L14">
         <f t="shared" si="2"/>
-        <v>3.7546974235700348</v>
+        <v>3.769558198109686</v>
       </c>
       <c r="M14">
         <f t="shared" si="3"/>
-        <v>3.9911505432125294</v>
+        <v>4.0068214977834424</v>
       </c>
       <c r="O14">
         <v>1.966</v>
@@ -33018,15 +32967,15 @@
       </c>
       <c r="J15">
         <f t="shared" si="1"/>
-        <v>3.8994429776952622</v>
+        <v>3.9192362442055906</v>
       </c>
       <c r="L15">
         <f t="shared" si="2"/>
-        <v>3.7830903393623974</v>
+        <v>3.8027984373334847</v>
       </c>
       <c r="M15">
         <f t="shared" si="3"/>
-        <v>4.015795616028127</v>
+        <v>4.0356740510776961</v>
       </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
@@ -33054,15 +33003,15 @@
       </c>
       <c r="J16">
         <f t="shared" si="1"/>
-        <v>3.8861305194304672</v>
+        <v>3.9114200629864793</v>
       </c>
       <c r="L16">
         <f t="shared" si="2"/>
-        <v>3.7688371779427374</v>
+        <v>3.7944299384142495</v>
       </c>
       <c r="M16">
         <f t="shared" si="3"/>
-        <v>4.0034238609181969</v>
+        <v>4.0284101875587091</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -33090,15 +33039,15 @@
       </c>
       <c r="J17">
         <f t="shared" si="1"/>
-        <v>3.8339154951268708</v>
+        <v>3.8652767189011992</v>
       </c>
       <c r="L17">
         <f t="shared" si="2"/>
-        <v>3.7129324640929489</v>
+        <v>3.7450259501644103</v>
       </c>
       <c r="M17">
         <f t="shared" si="3"/>
-        <v>3.9548985261607927</v>
+        <v>3.985527487637988</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
@@ -33110,15 +33059,15 @@
       </c>
       <c r="J18">
         <f t="shared" si="1"/>
-        <v>3.7461805630556881</v>
+        <v>3.7837790412611172</v>
       </c>
       <c r="L18">
         <f t="shared" si="2"/>
-        <v>3.6189978861149341</v>
+        <v>3.6577693720308768</v>
       </c>
       <c r="M18">
         <f t="shared" si="3"/>
-        <v>3.8733632399964417</v>
+        <v>3.9097887104913571</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -33146,15 +33095,15 @@
       </c>
       <c r="J19">
         <f t="shared" si="1"/>
-        <v>3.6277933756099721</v>
+        <v>3.6714817292894395</v>
       </c>
       <c r="L19">
         <f t="shared" si="2"/>
-        <v>3.4922450611204972</v>
+        <v>3.5375367536301869</v>
       </c>
       <c r="M19">
         <f t="shared" si="3"/>
-        <v>3.7633416900994474</v>
+        <v>3.8054267049486925</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
@@ -33182,15 +33131,15 @@
       </c>
       <c r="J20">
         <f t="shared" si="1"/>
-        <v>3.4840268438749247</v>
+        <v>3.5334809550512043</v>
       </c>
       <c r="L20">
         <f t="shared" si="2"/>
-        <v>3.3383195018582219</v>
+        <v>3.3897843797161058</v>
       </c>
       <c r="M20">
         <f t="shared" si="3"/>
-        <v>3.6297341858916279</v>
+        <v>3.6771775303863032</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -33218,15 +33167,15 @@
       </c>
       <c r="J21">
         <f t="shared" si="1"/>
-        <v>3.3197924773771881</v>
+        <v>3.3746251318715244</v>
       </c>
       <c r="L21">
         <f t="shared" si="2"/>
-        <v>3.1624797816663288</v>
+        <v>3.2197032688351337</v>
       </c>
       <c r="M21">
         <f t="shared" si="3"/>
-        <v>3.4771051730880473</v>
+        <v>3.529546994907915</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -33254,15 +33203,15 @@
       </c>
       <c r="J22">
         <f t="shared" si="1"/>
-        <v>3.1392767991603678</v>
+        <v>3.1991078818296601</v>
       </c>
       <c r="L22">
         <f t="shared" si="2"/>
-        <v>2.9692082574124035</v>
+        <v>3.031783378532289</v>
       </c>
       <c r="M22">
         <f t="shared" si="3"/>
-        <v>3.3093453409083327</v>
+        <v>3.3664323851270317</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -33290,15 +33239,15 @@
       </c>
       <c r="J23">
         <f>$R$3+$O$3*SQRT(1+(I23-$Q$3)^2/$P$3^2)</f>
-        <v>2.9458686203169457</v>
+        <v>3.0103584003922133</v>
       </c>
       <c r="L23">
         <f t="shared" si="2"/>
-        <v>2.7621332049986957</v>
+        <v>2.8296962227798845</v>
       </c>
       <c r="M23">
         <f t="shared" si="3"/>
-        <v>3.1296040356351962</v>
+        <v>3.1910205780045415</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
@@ -39066,7 +39015,7 @@
       </c>
       <c r="J159">
         <f>$R$159+$O$159*SQRT(1+(I159-$Q$159)^2/$P$159^2)</f>
-        <v>1.5452026497595297</v>
+        <v>1.5310308253843257</v>
       </c>
       <c r="L159">
         <f>$R$45+$O$45*SQRT(1+(I159-$Q$45)^2/$P$45^2)</f>
@@ -39074,19 +39023,19 @@
       </c>
       <c r="M159">
         <f>$R$46+$O$46*SQRT(1+(I159-$Q166)^2/$P$46^2)</f>
-        <v>5.5805398760815361</v>
+        <v>5.5468173718374452</v>
       </c>
       <c r="O159">
         <v>-0.128</v>
       </c>
       <c r="P159">
-        <v>8.18</v>
+        <v>10.284000000000001</v>
       </c>
       <c r="Q159">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="R159">
-        <v>2.3380000000000001</v>
+        <v>2.2029999999999998</v>
       </c>
       <c r="U159" s="1">
         <v>42661.695138888892</v>
@@ -39153,7 +39102,7 @@
       </c>
       <c r="J160">
         <f t="shared" ref="J160:J179" si="33">$R$159+$O$159*SQRT(1+(I160-$Q$159)^2/$P$159^2)</f>
-        <v>1.6376943283880874</v>
+        <v>1.6041735873137231</v>
       </c>
       <c r="L160">
         <f t="shared" ref="L160:L179" si="34">$R$45+$O$45*SQRT(1+(I160-$Q$45)^2/$P$45^2)</f>
@@ -39240,7 +39189,7 @@
       </c>
       <c r="J161">
         <f t="shared" si="33"/>
-        <v>1.7297581355862586</v>
+        <v>1.6768845057213064</v>
       </c>
       <c r="L161">
         <f t="shared" si="34"/>
@@ -39315,7 +39264,7 @@
       </c>
       <c r="J162">
         <f t="shared" si="33"/>
-        <v>1.8211653704042383</v>
+        <v>1.7489560660003618</v>
       </c>
       <c r="L162">
         <f t="shared" si="34"/>
@@ -39331,15 +39280,15 @@
       </c>
       <c r="P162">
         <f t="shared" ref="P162:R162" si="36">P159-_xlfn.T.DIST(P159,17,TRUE)*P160</f>
-        <v>1.14200094746099</v>
+        <v>3.2460000360848156</v>
       </c>
       <c r="Q162">
         <f t="shared" si="36"/>
-        <v>48.777000000000001</v>
+        <v>51.777000000000001</v>
       </c>
       <c r="R162">
         <f t="shared" si="36"/>
-        <v>2.2474659607229284</v>
+        <v>2.1129171835180167</v>
       </c>
       <c r="U162" s="1">
         <v>42662.57916666667</v>
@@ -39406,7 +39355,7 @@
       </c>
       <c r="J163">
         <f t="shared" si="33"/>
-        <v>1.9114936813323122</v>
+        <v>1.820027135979615</v>
       </c>
       <c r="L163">
         <f t="shared" si="34"/>
@@ -39422,15 +39371,15 @@
       </c>
       <c r="P163">
         <f t="shared" ref="P163:R163" si="37">P159+_xlfn.T.DIST(P159,17,TRUE)*P160</f>
-        <v>15.21799905253901</v>
+        <v>17.321999963915186</v>
       </c>
       <c r="Q163">
         <f t="shared" si="37"/>
-        <v>51.222999999999999</v>
+        <v>54.222999999999999</v>
       </c>
       <c r="R163">
         <f t="shared" si="37"/>
-        <v>2.4285340392770718</v>
+        <v>2.293082816481983</v>
       </c>
       <c r="U163" s="1">
         <v>42663.383333333331</v>
@@ -39497,7 +39446,7 @@
       </c>
       <c r="J164">
         <f t="shared" si="33"/>
-        <v>1.9998772675969128</v>
+        <v>1.8894167175335406</v>
       </c>
       <c r="L164">
         <f t="shared" si="34"/>
@@ -39556,7 +39505,7 @@
       </c>
       <c r="J165">
         <f t="shared" si="33"/>
-        <v>2.0842756194959033</v>
+        <v>1.9557052863459128</v>
       </c>
       <c r="L165">
         <f t="shared" si="34"/>
@@ -39572,15 +39521,15 @@
       </c>
       <c r="P165">
         <f t="shared" ref="P165:R165" si="38">P162</f>
-        <v>1.14200094746099</v>
+        <v>3.2460000360848156</v>
       </c>
       <c r="Q165">
         <f t="shared" si="38"/>
-        <v>48.777000000000001</v>
+        <v>51.777000000000001</v>
       </c>
       <c r="R165">
         <f t="shared" si="38"/>
-        <v>2.2474659607229284</v>
+        <v>2.1129171835180167</v>
       </c>
       <c r="U165" s="1">
         <v>42664.380555555559</v>
@@ -39631,7 +39580,7 @@
       </c>
       <c r="J166">
         <f t="shared" si="33"/>
-        <v>2.1589612412162196</v>
+        <v>2.015573172538109</v>
       </c>
       <c r="L166">
         <f t="shared" si="34"/>
@@ -39647,15 +39596,15 @@
       </c>
       <c r="P166">
         <f t="shared" ref="P166:R166" si="39">P163</f>
-        <v>15.21799905253901</v>
+        <v>17.321999963915186</v>
       </c>
       <c r="Q166">
         <f t="shared" si="39"/>
-        <v>51.222999999999999</v>
+        <v>54.222999999999999</v>
       </c>
       <c r="R166">
         <f t="shared" si="39"/>
-        <v>2.4285340392770718</v>
+        <v>2.293082816481983</v>
       </c>
       <c r="U166" s="1">
         <v>42665.450694444444</v>
@@ -39706,7 +39655,7 @@
       </c>
       <c r="J167">
         <f t="shared" si="33"/>
-        <v>2.2062296322321391</v>
+        <v>2.0606732779975716</v>
       </c>
       <c r="L167">
         <f t="shared" si="34"/>
@@ -39765,7 +39714,7 @@
       </c>
       <c r="J168">
         <f t="shared" si="33"/>
-        <v>2.1955158981264606</v>
+        <v>2.0743962837557239</v>
       </c>
       <c r="L168">
         <f t="shared" si="34"/>
@@ -39824,7 +39773,7 @@
       </c>
       <c r="J169">
         <f t="shared" si="33"/>
-        <v>2.1358373290096999</v>
+        <v>2.0481617755201427</v>
       </c>
       <c r="L169">
         <f t="shared" si="34"/>
@@ -39842,7 +39791,7 @@
       </c>
       <c r="J170">
         <f t="shared" si="33"/>
-        <v>2.0568105468063442</v>
+        <v>1.9966876746758306</v>
       </c>
       <c r="L170">
         <f t="shared" si="34"/>
@@ -39878,7 +39827,7 @@
       </c>
       <c r="J171">
         <f t="shared" si="33"/>
-        <v>1.9707194418119127</v>
+        <v>1.9340973869713949</v>
       </c>
       <c r="L171">
         <f t="shared" si="34"/>
@@ -39914,7 +39863,7 @@
       </c>
       <c r="J172">
         <f t="shared" si="33"/>
-        <v>1.8815438191362173</v>
+        <v>1.8665384198769313</v>
       </c>
       <c r="L172">
         <f t="shared" si="34"/>
@@ -39950,7 +39899,7 @@
       </c>
       <c r="J173">
         <f t="shared" si="33"/>
-        <v>1.7907896031097921</v>
+        <v>1.796480487065421</v>
       </c>
       <c r="L173">
         <f t="shared" si="34"/>
@@ -39986,7 +39935,7 @@
       </c>
       <c r="J174">
         <f t="shared" si="33"/>
-        <v>1.6991291768511267</v>
+        <v>1.7250211575952579</v>
       </c>
       <c r="L174">
         <f t="shared" si="34"/>
@@ -40022,7 +39971,7 @@
       </c>
       <c r="J175">
         <f t="shared" si="33"/>
-        <v>1.6069033062123106</v>
+        <v>1.6527061030059103</v>
       </c>
       <c r="L175">
         <f t="shared" si="34"/>
@@ -40058,7 +40007,7 @@
       </c>
       <c r="J176">
         <f t="shared" si="33"/>
-        <v>1.5143019002972915</v>
+        <v>1.5798331585813787</v>
       </c>
       <c r="L176">
         <f t="shared" si="34"/>
@@ -40094,7 +40043,7 @@
       </c>
       <c r="J177">
         <f t="shared" si="33"/>
-        <v>1.4214387745324335</v>
+        <v>1.5065774333705615</v>
       </c>
       <c r="L177">
         <f t="shared" si="34"/>
@@ -40112,7 +40061,7 @@
       </c>
       <c r="J178">
         <f t="shared" si="33"/>
-        <v>1.328386144410868</v>
+        <v>1.433048176656381</v>
       </c>
       <c r="L178">
         <f t="shared" si="34"/>
@@ -40148,7 +40097,7 @@
       </c>
       <c r="J179">
         <f t="shared" si="33"/>
-        <v>1.2351919788309982</v>
+        <v>1.3593169024319933</v>
       </c>
       <c r="L179">
         <f t="shared" si="34"/>
@@ -42828,7 +42777,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V4" sqref="V4"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42921,7 +42870,7 @@
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L23" si="0">$V$3+$S$3*SQRT(1+(K3-$U$3)^2/$T$3^2)</f>
-        <v>1.4391275155102359</v>
+        <v>1.3988835148375665</v>
       </c>
       <c r="N3">
         <f>$V$5+$S$5*SQRT(1+(K3-$U$5)^2/$T$5^2)</f>
@@ -42935,20 +42884,20 @@
         <v>-1.766</v>
       </c>
       <c r="T3">
-        <v>40.017000000000003</v>
+        <v>39.915999999999997</v>
       </c>
       <c r="U3">
-        <v>73</v>
+        <v>73.8</v>
       </c>
       <c r="V3">
-        <v>5.1130000000000004</v>
+        <v>5.1109999999999998</v>
       </c>
       <c r="X3">
         <v>0</v>
       </c>
       <c r="Y3">
         <f>$V$3-$S$3/$T$3*X3+$S$3/$T$3*$U$3</f>
-        <v>1.8914191718519637</v>
+        <v>1.8458732337909605</v>
       </c>
       <c r="AA3">
         <f>$V$7-$S$7/$T$7*X3+$S$7/$T$7*$U$7</f>
@@ -42980,7 +42929,7 @@
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1.6689641421115926</v>
+        <v>1.6300846113976495</v>
       </c>
       <c r="N4">
         <f t="shared" ref="N4:N23" si="2">$V$5+$S$5*SQRT(1+(K4-$U$5)^2/$T$5^2)</f>
@@ -42995,7 +42944,7 @@
       </c>
       <c r="Y4">
         <f t="shared" ref="Y4:Y23" si="4">$V$3-$S$3/$T$3*X4+$S$3/$T$3*$U$3</f>
-        <v>2.1562066371791992</v>
+        <v>2.1113306944583621</v>
       </c>
       <c r="AA4">
         <f t="shared" ref="AA4:AA23" si="5">$V$7-$S$7/$T$7*X4+$S$7/$T$7*$U$7</f>
@@ -43030,7 +42979,7 @@
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1.893426774844198</v>
+        <v>1.8560544685585634</v>
       </c>
       <c r="N5">
         <f t="shared" si="2"/>
@@ -43057,7 +43006,7 @@
       </c>
       <c r="Y5">
         <f t="shared" si="4"/>
-        <v>2.4209941025064357</v>
+        <v>2.3767881551257637</v>
       </c>
       <c r="AA5">
         <f t="shared" si="5"/>
@@ -43089,7 +43038,7 @@
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>2.1113095900063295</v>
+        <v>2.0756245356561784</v>
       </c>
       <c r="N6">
         <f t="shared" si="2"/>
@@ -43104,7 +43053,7 @@
       </c>
       <c r="Y6">
         <f t="shared" si="4"/>
-        <v>2.6857815678336712</v>
+        <v>2.6422456157931653</v>
       </c>
       <c r="AA6">
         <f t="shared" si="5"/>
@@ -43139,7 +43088,7 @@
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>2.3210716903285906</v>
+        <v>2.2873014797471156</v>
       </c>
       <c r="N7">
         <f t="shared" si="2"/>
@@ -43166,7 +43115,7 @@
       </c>
       <c r="Y7">
         <f t="shared" si="4"/>
-        <v>2.9505690331609076</v>
+        <v>2.9077030764605669</v>
       </c>
       <c r="AA7">
         <f t="shared" si="5"/>
@@ -43198,7 +43147,7 @@
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>2.5207409738164319</v>
+        <v>2.48917281578969</v>
       </c>
       <c r="N8">
         <f t="shared" si="2"/>
@@ -43213,7 +43162,7 @@
       </c>
       <c r="Y8">
         <f t="shared" si="4"/>
-        <v>3.2153564984881431</v>
+        <v>3.1731605371279685</v>
       </c>
       <c r="AA8">
         <f t="shared" si="5"/>
@@ -43231,7 +43180,7 @@
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>2.7078025372322232</v>
+        <v>2.678795740218769</v>
       </c>
       <c r="N9">
         <f t="shared" si="2"/>
@@ -43246,7 +43195,7 @@
       </c>
       <c r="Y9">
         <f t="shared" si="4"/>
-        <v>3.4801439638153795</v>
+        <v>3.4386179977953701</v>
       </c>
       <c r="AA9">
         <f t="shared" si="5"/>
@@ -43278,7 +43227,7 @@
       </c>
       <c r="L10">
         <f t="shared" si="0"/>
-        <v>2.8790869277056084</v>
+        <v>2.853082227896742</v>
       </c>
       <c r="N10">
         <f t="shared" si="2"/>
@@ -43293,7 +43242,7 @@
       </c>
       <c r="Y10">
         <f t="shared" si="4"/>
-        <v>3.744931429142615</v>
+        <v>3.7040754584627718</v>
       </c>
       <c r="AA10">
         <f t="shared" si="5"/>
@@ -43325,7 +43274,7 @@
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>3.0306971407069945</v>
+        <v>3.008215394599465</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
@@ -43340,7 +43289,7 @@
       </c>
       <c r="Y11">
         <f t="shared" si="4"/>
-        <v>4.0097188944698505</v>
+        <v>3.9695329191301725</v>
       </c>
       <c r="AA11">
         <f t="shared" si="5"/>
@@ -43372,7 +43321,7 @@
       </c>
       <c r="L12">
         <f t="shared" si="0"/>
-        <v>3.1580504905085829</v>
+        <v>3.1396682535181455</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
@@ -43387,7 +43336,7 @@
       </c>
       <c r="Y12">
         <f t="shared" si="4"/>
-        <v>4.2745063597970869</v>
+        <v>4.2349903797975745</v>
       </c>
       <c r="AA12">
         <f t="shared" si="5"/>
@@ -43419,7 +43368,7 @@
       </c>
       <c r="L13">
         <f t="shared" si="0"/>
-        <v>3.256149231873902</v>
+        <v>3.2424363967172853</v>
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
@@ -43434,7 +43383,7 @@
       </c>
       <c r="Y13">
         <f t="shared" si="4"/>
-        <v>4.5392938251243233</v>
+        <v>4.5004478404649753</v>
       </c>
       <c r="AA13">
         <f t="shared" si="5"/>
@@ -43466,7 +43415,7 @@
       </c>
       <c r="L14">
         <f t="shared" si="0"/>
-        <v>3.3201846807021438</v>
+        <v>3.3115983352273637</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
@@ -43481,7 +43430,7 @@
       </c>
       <c r="Y14">
         <f t="shared" si="4"/>
-        <v>4.804081290451558</v>
+        <v>4.7659053011323778</v>
       </c>
       <c r="AA14">
         <f t="shared" si="5"/>
@@ -43513,7 +43462,7 @@
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>3.3464486798520374</v>
+        <v>3.3432053032922178</v>
       </c>
       <c r="N15">
         <f t="shared" si="2"/>
@@ -43528,7 +43477,7 @@
       </c>
       <c r="Y15">
         <f t="shared" si="4"/>
-        <v>5.0688687557787944</v>
+        <v>5.0313627617997785</v>
       </c>
       <c r="AA15">
         <f t="shared" si="5"/>
@@ -43545,7 +43494,7 @@
       </c>
       <c r="L16">
         <f t="shared" si="0"/>
-        <v>3.3332682314705986</v>
+        <v>3.3352508186464638</v>
       </c>
       <c r="N16">
         <f t="shared" si="2"/>
@@ -43560,7 +43509,7 @@
       </c>
       <c r="Y16">
         <f t="shared" si="4"/>
-        <v>5.3336562211060308</v>
+        <v>5.296820222467181</v>
       </c>
       <c r="AA16">
         <f t="shared" si="5"/>
@@ -43592,7 +43541,7 @@
       </c>
       <c r="L17">
         <f t="shared" si="0"/>
-        <v>3.28149472490579</v>
+        <v>3.2882527472808203</v>
       </c>
       <c r="N17">
         <f t="shared" si="2"/>
@@ -43607,7 +43556,7 @@
       </c>
       <c r="Y17">
         <f t="shared" si="4"/>
-        <v>5.5984436864332654</v>
+        <v>5.5622776831345817</v>
       </c>
       <c r="AA17">
         <f t="shared" si="5"/>
@@ -43639,7 +43588,7 @@
       </c>
       <c r="L18">
         <f t="shared" si="0"/>
-        <v>3.1942496824568636</v>
+        <v>3.2050972568462859</v>
       </c>
       <c r="N18">
         <f t="shared" si="2"/>
@@ -43654,7 +43603,7 @@
       </c>
       <c r="Y18">
         <f t="shared" si="4"/>
-        <v>5.8632311517605018</v>
+        <v>5.8277351438019842</v>
       </c>
       <c r="AA18">
         <f t="shared" si="5"/>
@@ -43686,7 +43635,7 @@
       </c>
       <c r="L19">
         <f t="shared" si="0"/>
-        <v>3.0760859632682824</v>
+        <v>3.0902431338049703</v>
       </c>
       <c r="N19">
         <f t="shared" si="2"/>
@@ -43701,7 +43650,7 @@
       </c>
       <c r="Y19">
         <f t="shared" si="4"/>
-        <v>6.1280186170877382</v>
+        <v>6.0931926044693849</v>
       </c>
       <c r="AA19">
         <f t="shared" si="5"/>
@@ -43733,7 +43682,7 @@
       </c>
       <c r="L20">
         <f t="shared" si="0"/>
-        <v>2.932023244372751</v>
+        <v>2.9487357504144338</v>
       </c>
       <c r="N20">
         <f t="shared" si="2"/>
@@ -43748,7 +43697,7 @@
       </c>
       <c r="Y20">
         <f t="shared" si="4"/>
-        <v>6.3928060824149728</v>
+        <v>6.3586500651367857</v>
       </c>
       <c r="AA20">
         <f t="shared" si="5"/>
@@ -43780,7 +43729,7 @@
       </c>
       <c r="L21">
         <f t="shared" si="0"/>
-        <v>2.766827536661709</v>
+        <v>2.7854354696879993</v>
       </c>
       <c r="N21">
         <f t="shared" si="2"/>
@@ -43795,7 +43744,7 @@
       </c>
       <c r="Y21">
         <f t="shared" si="4"/>
-        <v>6.657593547742211</v>
+        <v>6.6241075258041882</v>
       </c>
       <c r="AA21">
         <f t="shared" si="5"/>
@@ -43827,7 +43776,7 @@
       </c>
       <c r="L22">
         <f t="shared" si="0"/>
-        <v>2.5846377533161493</v>
+        <v>2.604598314095945</v>
       </c>
       <c r="N22">
         <f t="shared" si="2"/>
@@ -43842,7 +43791,7 @@
       </c>
       <c r="Y22">
         <f t="shared" si="4"/>
-        <v>6.9223810130694456</v>
+        <v>6.8895649864715907</v>
       </c>
       <c r="AA22">
         <f t="shared" si="5"/>
@@ -43855,7 +43804,7 @@
       </c>
       <c r="L23">
         <f t="shared" si="0"/>
-        <v>2.3888614431761361</v>
+        <v>2.4097440394497833</v>
       </c>
       <c r="N23">
         <f t="shared" si="2"/>
@@ -43870,7 +43819,7 @@
       </c>
       <c r="Y23">
         <f t="shared" si="4"/>
-        <v>7.187168478396682</v>
+        <v>7.1550224471389914</v>
       </c>
       <c r="AA23">
         <f t="shared" si="5"/>

</xml_diff>